<commit_message>
Actualizaciones al código y a la base de datos.
</commit_message>
<xml_diff>
--- a/datos_Iniciales1.xlsx
+++ b/datos_Iniciales1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanlinares/Desktop/Proyecto_simulacion_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BA73ED-FCF2-5549-B531-4ACF12F66D73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D28E6B-1E9E-374D-9EAF-ABFB61E8CE46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{E1880CBD-E780-9541-AEB9-7B512A2078D9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{E1880CBD-E780-9541-AEB9-7B512A2078D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>S</t>
   </si>
@@ -157,13 +157,24 @@
   </si>
   <si>
     <t>Beta_Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>NACIONAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.000000000_-;\-* #,##0.000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0000000000000_-;\-* #,##0.0000000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -174,6 +185,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -196,16 +214,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -518,15 +543,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A98531-A01F-1241-AFA9-7F25A9E017A6}">
-  <dimension ref="A1:AG10"/>
+  <dimension ref="A1:AH15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="AF15" sqref="AF15"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -623,8 +652,11 @@
       <c r="AG1" t="s">
         <v>32</v>
       </c>
+      <c r="AH1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -724,8 +756,12 @@
       <c r="AG2">
         <v>0.39707325737836546</v>
       </c>
+      <c r="AH2">
+        <f>0.4*(1-AH3-AH4-AH5-AH7)</f>
+        <v>0.39682279726962555</v>
+      </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -825,8 +861,12 @@
       <c r="AG3">
         <v>4.5846620251964383E-4</v>
       </c>
+      <c r="AH3" s="4">
+        <f>25136/AH11</f>
+        <v>1.9669418856784517E-4</v>
+      </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -839,7 +879,7 @@
       <c r="D4">
         <v>1.093564373661005E-4</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>0</v>
       </c>
       <c r="F4">
@@ -926,8 +966,12 @@
       <c r="AG4">
         <v>1.3922010338292851E-4</v>
       </c>
+      <c r="AH4">
+        <f>(80/20)*AH5</f>
+        <v>1.9253118298548944E-4</v>
+      </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1027,8 +1071,12 @@
       <c r="AG5">
         <v>3.4805025845732126E-5</v>
       </c>
+      <c r="AH5" s="4">
+        <f>6151/AH11</f>
+        <v>4.8132795746372359E-5</v>
+      </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1128,8 +1176,12 @@
       <c r="AG6">
         <v>0.59560988606754817</v>
       </c>
+      <c r="AH6" s="4">
+        <f>0.6*(1-AH3-AH4-AH5-AH7)</f>
+        <v>0.59523419590443827</v>
+      </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1229,8 +1281,12 @@
       <c r="AG7">
         <v>6.6843652223381057E-3</v>
       </c>
+      <c r="AH7" s="4">
+        <f>959164/AH11</f>
+        <v>7.505648658636563E-3</v>
+      </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1330,8 +1386,11 @@
       <c r="AG8" s="1">
         <v>0.74011298999999997</v>
       </c>
+      <c r="AH8">
+        <v>0.84943570000000002</v>
+      </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1431,8 +1490,11 @@
       <c r="AG9">
         <v>0.12024535682050499</v>
       </c>
+      <c r="AH9">
+        <v>0.13800689925236548</v>
+      </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1532,6 +1594,118 @@
       <c r="AG10">
         <v>0.218627921491827</v>
       </c>
+      <c r="AH10">
+        <v>0.25092163500430087</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11">
+        <v>1434635</v>
+      </c>
+      <c r="C11">
+        <v>3634868</v>
+      </c>
+      <c r="D11">
+        <v>804708</v>
+      </c>
+      <c r="E11">
+        <v>1000617</v>
+      </c>
+      <c r="F11">
+        <v>5730367</v>
+      </c>
+      <c r="G11">
+        <v>3801487</v>
+      </c>
+      <c r="H11">
+        <v>9018645</v>
+      </c>
+      <c r="I11">
+        <v>3218720</v>
+      </c>
+      <c r="J11">
+        <v>785153</v>
+      </c>
+      <c r="K11">
+        <v>1868996</v>
+      </c>
+      <c r="L11">
+        <v>6228175</v>
+      </c>
+      <c r="M11">
+        <v>3657048</v>
+      </c>
+      <c r="N11">
+        <v>3086414</v>
+      </c>
+      <c r="O11">
+        <v>8409693</v>
+      </c>
+      <c r="P11">
+        <v>17427790</v>
+      </c>
+      <c r="Q11">
+        <v>4825401</v>
+      </c>
+      <c r="R11">
+        <v>2044058</v>
+      </c>
+      <c r="S11">
+        <v>1288571</v>
+      </c>
+      <c r="T11">
+        <v>5610153</v>
+      </c>
+      <c r="U11">
+        <v>4143593</v>
+      </c>
+      <c r="V11">
+        <v>6604451</v>
+      </c>
+      <c r="W11">
+        <v>2279637</v>
+      </c>
+      <c r="X11">
+        <v>1723259</v>
+      </c>
+      <c r="Y11">
+        <v>2866142</v>
+      </c>
+      <c r="Z11">
+        <v>3156674</v>
+      </c>
+      <c r="AA11">
+        <v>3074745</v>
+      </c>
+      <c r="AB11">
+        <v>2572287</v>
+      </c>
+      <c r="AC11">
+        <v>3650602</v>
+      </c>
+      <c r="AD11">
+        <v>1380011</v>
+      </c>
+      <c r="AE11">
+        <v>8539862</v>
+      </c>
+      <c r="AF11">
+        <v>2259098</v>
+      </c>
+      <c r="AG11">
+        <v>1666426</v>
+      </c>
+      <c r="AH11" s="2">
+        <f>SUM(B11:AG11)</f>
+        <v>127792286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="D15" s="5"/>
+      <c r="E15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>